<commit_message>
[IMP] z0bug_odoo invoice data
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice_line.xlsx
+++ b/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice_line.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Special service for Young people</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_512000</t>
+    <t xml:space="preserve">external.512000</t>
   </si>
   <si>
     <t xml:space="preserve">0.71</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Sviluppo prototipo Powerp</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_510200</t>
+    <t xml:space="preserve">external.510200</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;2-12-01</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Prodotto Alpha</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_510000</t>
+    <t xml:space="preserve">external.510000</t>
   </si>
   <si>
     <t xml:space="preserve">0.84</t>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">Prodotto Rho</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_510100</t>
+    <t xml:space="preserve">external.510100</t>
   </si>
   <si>
     <t xml:space="preserve">1.19</t>
@@ -559,7 +559,7 @@
     <t xml:space="preserve">Costituzione società</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_623460</t>
+    <t xml:space="preserve">external.623460</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_22a</t>
@@ -577,7 +577,7 @@
     <t xml:space="preserve">PC Nico</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_123380</t>
+    <t xml:space="preserve">external.123380</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_ZI_2_1</t>
@@ -586,7 +586,7 @@
     <t xml:space="preserve">z0bug.invoice_ZI_2</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.coa_610100</t>
+    <t xml:space="preserve">external.610100</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_2220</t>
@@ -843,9 +843,9 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="G32" activeCellId="0" sqref="G2:G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>